<commit_message>
feedback, get feedbacks about note, media
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,13 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="1" r:id="rId1"/>
     <sheet name="Account" sheetId="2" r:id="rId2"/>
     <sheet name="Context" sheetId="3" r:id="rId3"/>
+    <sheet name="Feedback" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Feedback!$F$1:$F$101</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="178">
   <si>
     <t>tomyeh</t>
   </si>
@@ -498,6 +502,63 @@
   </si>
   <si>
     <t>many birds live here</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>a very interenting person</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>an interesting note</t>
+  </si>
+  <si>
+    <t>Context</t>
+  </si>
+  <si>
+    <t>very fine activity</t>
+  </si>
+  <si>
+    <t>great</t>
+  </si>
+  <si>
+    <t>I love this</t>
+  </si>
+  <si>
+    <t>This is terrible</t>
+  </si>
+  <si>
+    <t>I don't like this</t>
+  </si>
+  <si>
+    <t>This is fun</t>
+  </si>
+  <si>
+    <t>What is this?</t>
+  </si>
+  <si>
+    <t>I don't understand</t>
+  </si>
+  <si>
+    <t>What is the point</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Media</t>
   </si>
 </sst>
 </file>
@@ -557,7 +618,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="86">
+  <cellStyleXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -643,13 +704,55 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="86">
+  <cellStyles count="128">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -719,6 +822,27 @@
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -735,6 +859,27 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1066,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4096,4 +4241,2152 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <f t="shared" ref="A4:A7" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <f>A7+1</f>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <f>A8+1</f>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <f>A9+1</f>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <f>A10+1</f>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" t="s">
+        <v>162</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <f>A11+1</f>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>161</v>
+      </c>
+      <c r="E12" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <f>A12+1</f>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" t="s">
+        <v>167</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <f>A13+1</f>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" t="s">
+        <v>167</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <f>A14+1</f>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <f>A15+1</f>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>161</v>
+      </c>
+      <c r="E16" t="s">
+        <v>165</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <f>A16+1</f>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" t="s">
+        <v>167</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <f>A17+1</f>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>161</v>
+      </c>
+      <c r="E18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <f>A18+1</f>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>161</v>
+      </c>
+      <c r="E19" t="s">
+        <v>162</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <f>A19+1</f>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>161</v>
+      </c>
+      <c r="E20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <f>A20+1</f>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>161</v>
+      </c>
+      <c r="E21" t="s">
+        <v>167</v>
+      </c>
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <f>A21+1</f>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>161</v>
+      </c>
+      <c r="E22" t="s">
+        <v>167</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <f>A22+1</f>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" t="s">
+        <v>162</v>
+      </c>
+      <c r="F23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <f>A23+1</f>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>161</v>
+      </c>
+      <c r="E24" t="s">
+        <v>165</v>
+      </c>
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <f>A24+1</f>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" t="s">
+        <v>167</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <f>A25+1</f>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>161</v>
+      </c>
+      <c r="E26" t="s">
+        <v>167</v>
+      </c>
+      <c r="F26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <f>A26+1</f>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>163</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>161</v>
+      </c>
+      <c r="E27" t="s">
+        <v>162</v>
+      </c>
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <f>A27+1</f>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>161</v>
+      </c>
+      <c r="E28" t="s">
+        <v>165</v>
+      </c>
+      <c r="F28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <f>A28+1</f>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>166</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>161</v>
+      </c>
+      <c r="E29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <f>A29+1</f>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>164</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>161</v>
+      </c>
+      <c r="E30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <f>A30+1</f>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>161</v>
+      </c>
+      <c r="E31" t="s">
+        <v>169</v>
+      </c>
+      <c r="F31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <f>A31+1</f>
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>164</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>161</v>
+      </c>
+      <c r="E32" t="s">
+        <v>168</v>
+      </c>
+      <c r="F32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <f>A32+1</f>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>161</v>
+      </c>
+      <c r="E33" t="s">
+        <v>170</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <f>A33+1</f>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>161</v>
+      </c>
+      <c r="E34" t="s">
+        <v>171</v>
+      </c>
+      <c r="F34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <f>A34+1</f>
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <f>A35+1</f>
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>161</v>
+      </c>
+      <c r="E36" t="s">
+        <v>169</v>
+      </c>
+      <c r="F36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <f>A36+1</f>
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>161</v>
+      </c>
+      <c r="E37" t="s">
+        <v>168</v>
+      </c>
+      <c r="F37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <f>A37+1</f>
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>164</v>
+      </c>
+      <c r="C38">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>161</v>
+      </c>
+      <c r="E38" t="s">
+        <v>170</v>
+      </c>
+      <c r="F38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <f>A38+1</f>
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>164</v>
+      </c>
+      <c r="C39">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
+        <v>161</v>
+      </c>
+      <c r="E39" t="s">
+        <v>171</v>
+      </c>
+      <c r="F39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <f>A39+1</f>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40">
+        <v>13</v>
+      </c>
+      <c r="D40" t="s">
+        <v>161</v>
+      </c>
+      <c r="E40" t="s">
+        <v>169</v>
+      </c>
+      <c r="F40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
+        <f>A40+1</f>
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41">
+        <v>14</v>
+      </c>
+      <c r="D41" t="s">
+        <v>161</v>
+      </c>
+      <c r="E41" t="s">
+        <v>168</v>
+      </c>
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <f>A41+1</f>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>164</v>
+      </c>
+      <c r="C42">
+        <v>15</v>
+      </c>
+      <c r="D42" t="s">
+        <v>161</v>
+      </c>
+      <c r="E42" t="s">
+        <v>172</v>
+      </c>
+      <c r="F42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <f>A42+1</f>
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43">
+        <v>16</v>
+      </c>
+      <c r="D43" t="s">
+        <v>161</v>
+      </c>
+      <c r="E43" t="s">
+        <v>173</v>
+      </c>
+      <c r="F43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
+        <f>A43+1</f>
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C44">
+        <v>17</v>
+      </c>
+      <c r="D44" t="s">
+        <v>161</v>
+      </c>
+      <c r="E44" t="s">
+        <v>171</v>
+      </c>
+      <c r="F44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <f>A44+1</f>
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45">
+        <v>18</v>
+      </c>
+      <c r="D45" t="s">
+        <v>161</v>
+      </c>
+      <c r="E45" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <f>A45+1</f>
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46">
+        <v>19</v>
+      </c>
+      <c r="D46" t="s">
+        <v>161</v>
+      </c>
+      <c r="E46" t="s">
+        <v>169</v>
+      </c>
+      <c r="F46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <f>A46+1</f>
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47">
+        <v>20</v>
+      </c>
+      <c r="D47" t="s">
+        <v>161</v>
+      </c>
+      <c r="E47" t="s">
+        <v>168</v>
+      </c>
+      <c r="F47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <f>A47+1</f>
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>164</v>
+      </c>
+      <c r="C48">
+        <v>21</v>
+      </c>
+      <c r="D48" t="s">
+        <v>161</v>
+      </c>
+      <c r="E48" t="s">
+        <v>170</v>
+      </c>
+      <c r="F48" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <f>A48+1</f>
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>164</v>
+      </c>
+      <c r="C49">
+        <v>22</v>
+      </c>
+      <c r="D49" t="s">
+        <v>161</v>
+      </c>
+      <c r="E49" t="s">
+        <v>171</v>
+      </c>
+      <c r="F49" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <f>A49+1</f>
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C50">
+        <v>23</v>
+      </c>
+      <c r="D50" t="s">
+        <v>161</v>
+      </c>
+      <c r="E50" t="s">
+        <v>169</v>
+      </c>
+      <c r="F50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <f>A50+1</f>
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51">
+        <v>24</v>
+      </c>
+      <c r="D51" t="s">
+        <v>161</v>
+      </c>
+      <c r="E51" t="s">
+        <v>168</v>
+      </c>
+      <c r="F51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <f>A51+1</f>
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>164</v>
+      </c>
+      <c r="C52">
+        <v>25</v>
+      </c>
+      <c r="D52" t="s">
+        <v>161</v>
+      </c>
+      <c r="E52" t="s">
+        <v>172</v>
+      </c>
+      <c r="F52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
+        <f>A52+1</f>
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>164</v>
+      </c>
+      <c r="C53">
+        <v>26</v>
+      </c>
+      <c r="D53" t="s">
+        <v>161</v>
+      </c>
+      <c r="E53" t="s">
+        <v>173</v>
+      </c>
+      <c r="F53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
+        <f>A53+1</f>
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>164</v>
+      </c>
+      <c r="C54">
+        <v>27</v>
+      </c>
+      <c r="D54" t="s">
+        <v>161</v>
+      </c>
+      <c r="E54" t="s">
+        <v>169</v>
+      </c>
+      <c r="F54" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <f>A54+1</f>
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>164</v>
+      </c>
+      <c r="C55">
+        <v>28</v>
+      </c>
+      <c r="D55" t="s">
+        <v>161</v>
+      </c>
+      <c r="E55" t="s">
+        <v>174</v>
+      </c>
+      <c r="F55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <f>A55+1</f>
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56">
+        <v>29</v>
+      </c>
+      <c r="D56" t="s">
+        <v>161</v>
+      </c>
+      <c r="E56" t="s">
+        <v>172</v>
+      </c>
+      <c r="F56" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <f>A56+1</f>
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>164</v>
+      </c>
+      <c r="C57">
+        <v>30</v>
+      </c>
+      <c r="D57" t="s">
+        <v>161</v>
+      </c>
+      <c r="E57" t="s">
+        <v>173</v>
+      </c>
+      <c r="F57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
+        <f>A57+1</f>
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>164</v>
+      </c>
+      <c r="C58">
+        <v>31</v>
+      </c>
+      <c r="D58" t="s">
+        <v>161</v>
+      </c>
+      <c r="E58" t="s">
+        <v>171</v>
+      </c>
+      <c r="F58" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59">
+        <f>A58+1</f>
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C59">
+        <v>32</v>
+      </c>
+      <c r="D59" t="s">
+        <v>161</v>
+      </c>
+      <c r="E59" t="s">
+        <v>43</v>
+      </c>
+      <c r="F59" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
+        <f>A59+1</f>
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>164</v>
+      </c>
+      <c r="C60">
+        <v>33</v>
+      </c>
+      <c r="D60" t="s">
+        <v>161</v>
+      </c>
+      <c r="E60" t="s">
+        <v>169</v>
+      </c>
+      <c r="F60" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
+        <f>A60+1</f>
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>164</v>
+      </c>
+      <c r="C61">
+        <v>34</v>
+      </c>
+      <c r="D61" t="s">
+        <v>161</v>
+      </c>
+      <c r="E61" t="s">
+        <v>168</v>
+      </c>
+      <c r="F61" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
+        <f>A61+1</f>
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>164</v>
+      </c>
+      <c r="C62">
+        <v>35</v>
+      </c>
+      <c r="D62" t="s">
+        <v>161</v>
+      </c>
+      <c r="E62" t="s">
+        <v>170</v>
+      </c>
+      <c r="F62" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
+        <f>A62+1</f>
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>164</v>
+      </c>
+      <c r="C63">
+        <v>36</v>
+      </c>
+      <c r="D63" t="s">
+        <v>161</v>
+      </c>
+      <c r="E63" t="s">
+        <v>171</v>
+      </c>
+      <c r="F63" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64">
+        <f>A63+1</f>
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>164</v>
+      </c>
+      <c r="C64">
+        <v>37</v>
+      </c>
+      <c r="D64" t="s">
+        <v>161</v>
+      </c>
+      <c r="E64" t="s">
+        <v>169</v>
+      </c>
+      <c r="F64" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65">
+        <f>A64+1</f>
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>164</v>
+      </c>
+      <c r="C65">
+        <v>38</v>
+      </c>
+      <c r="D65" t="s">
+        <v>161</v>
+      </c>
+      <c r="E65" t="s">
+        <v>168</v>
+      </c>
+      <c r="F65" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66">
+        <f>A65+1</f>
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>164</v>
+      </c>
+      <c r="C66">
+        <v>39</v>
+      </c>
+      <c r="D66" t="s">
+        <v>161</v>
+      </c>
+      <c r="E66" t="s">
+        <v>172</v>
+      </c>
+      <c r="F66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67">
+        <f>A66+1</f>
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>164</v>
+      </c>
+      <c r="C67">
+        <v>40</v>
+      </c>
+      <c r="D67" t="s">
+        <v>161</v>
+      </c>
+      <c r="E67" t="s">
+        <v>173</v>
+      </c>
+      <c r="F67" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>164</v>
+      </c>
+      <c r="C68">
+        <v>41</v>
+      </c>
+      <c r="D68" t="s">
+        <v>161</v>
+      </c>
+      <c r="E68" t="s">
+        <v>175</v>
+      </c>
+      <c r="F68" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69">
+        <f>A68+1</f>
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>164</v>
+      </c>
+      <c r="C69">
+        <v>12</v>
+      </c>
+      <c r="D69" t="s">
+        <v>161</v>
+      </c>
+      <c r="E69" t="s">
+        <v>171</v>
+      </c>
+      <c r="F69" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70">
+        <f>A69+1</f>
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>164</v>
+      </c>
+      <c r="C70">
+        <v>13</v>
+      </c>
+      <c r="D70" t="s">
+        <v>161</v>
+      </c>
+      <c r="E70" t="s">
+        <v>169</v>
+      </c>
+      <c r="F70" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71">
+        <f>A70+1</f>
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>164</v>
+      </c>
+      <c r="C71">
+        <v>14</v>
+      </c>
+      <c r="D71" t="s">
+        <v>161</v>
+      </c>
+      <c r="E71" t="s">
+        <v>168</v>
+      </c>
+      <c r="F71" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72">
+        <f>A71+1</f>
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>164</v>
+      </c>
+      <c r="C72">
+        <v>15</v>
+      </c>
+      <c r="D72" t="s">
+        <v>161</v>
+      </c>
+      <c r="E72" t="s">
+        <v>172</v>
+      </c>
+      <c r="F72" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73">
+        <f>A72+1</f>
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>164</v>
+      </c>
+      <c r="C73">
+        <v>16</v>
+      </c>
+      <c r="D73" t="s">
+        <v>161</v>
+      </c>
+      <c r="E73" t="s">
+        <v>173</v>
+      </c>
+      <c r="F73" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74">
+        <f>A73+1</f>
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>164</v>
+      </c>
+      <c r="C74">
+        <v>17</v>
+      </c>
+      <c r="D74" t="s">
+        <v>161</v>
+      </c>
+      <c r="E74" t="s">
+        <v>171</v>
+      </c>
+      <c r="F74" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75">
+        <f>A74+1</f>
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>164</v>
+      </c>
+      <c r="C75">
+        <v>18</v>
+      </c>
+      <c r="D75" t="s">
+        <v>161</v>
+      </c>
+      <c r="E75" t="s">
+        <v>43</v>
+      </c>
+      <c r="F75" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76">
+        <f>A75+1</f>
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>164</v>
+      </c>
+      <c r="C76">
+        <v>19</v>
+      </c>
+      <c r="D76" t="s">
+        <v>161</v>
+      </c>
+      <c r="E76" t="s">
+        <v>169</v>
+      </c>
+      <c r="F76" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77">
+        <f>A76+1</f>
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>164</v>
+      </c>
+      <c r="C77">
+        <v>20</v>
+      </c>
+      <c r="D77" t="s">
+        <v>161</v>
+      </c>
+      <c r="E77" t="s">
+        <v>168</v>
+      </c>
+      <c r="F77" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78">
+        <f>A77+1</f>
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>164</v>
+      </c>
+      <c r="C78">
+        <v>21</v>
+      </c>
+      <c r="D78" t="s">
+        <v>161</v>
+      </c>
+      <c r="E78" t="s">
+        <v>170</v>
+      </c>
+      <c r="F78" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79">
+        <f>A78+1</f>
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>164</v>
+      </c>
+      <c r="C79">
+        <v>22</v>
+      </c>
+      <c r="D79" t="s">
+        <v>161</v>
+      </c>
+      <c r="E79" t="s">
+        <v>171</v>
+      </c>
+      <c r="F79" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80">
+        <f>A79+1</f>
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>164</v>
+      </c>
+      <c r="C80">
+        <v>23</v>
+      </c>
+      <c r="D80" t="s">
+        <v>161</v>
+      </c>
+      <c r="E80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F80" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81">
+        <f>A80+1</f>
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>164</v>
+      </c>
+      <c r="C81">
+        <v>24</v>
+      </c>
+      <c r="D81" t="s">
+        <v>161</v>
+      </c>
+      <c r="E81" t="s">
+        <v>168</v>
+      </c>
+      <c r="F81" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82">
+        <f>A81+1</f>
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>164</v>
+      </c>
+      <c r="C82">
+        <v>25</v>
+      </c>
+      <c r="D82" t="s">
+        <v>161</v>
+      </c>
+      <c r="E82" t="s">
+        <v>172</v>
+      </c>
+      <c r="F82" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83">
+        <f>A82+1</f>
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>164</v>
+      </c>
+      <c r="C83">
+        <v>26</v>
+      </c>
+      <c r="D83" t="s">
+        <v>161</v>
+      </c>
+      <c r="E83" t="s">
+        <v>173</v>
+      </c>
+      <c r="F83" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84">
+        <f>A83+1</f>
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>164</v>
+      </c>
+      <c r="C84">
+        <v>27</v>
+      </c>
+      <c r="D84" t="s">
+        <v>161</v>
+      </c>
+      <c r="E84" t="s">
+        <v>169</v>
+      </c>
+      <c r="F84" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85">
+        <f>A84+1</f>
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>164</v>
+      </c>
+      <c r="C85">
+        <v>28</v>
+      </c>
+      <c r="D85" t="s">
+        <v>161</v>
+      </c>
+      <c r="E85" t="s">
+        <v>174</v>
+      </c>
+      <c r="F85" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86">
+        <f>A85+1</f>
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>164</v>
+      </c>
+      <c r="C86">
+        <v>29</v>
+      </c>
+      <c r="D86" t="s">
+        <v>161</v>
+      </c>
+      <c r="E86" t="s">
+        <v>172</v>
+      </c>
+      <c r="F86" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87">
+        <f>A86+1</f>
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>164</v>
+      </c>
+      <c r="C87">
+        <v>30</v>
+      </c>
+      <c r="D87" t="s">
+        <v>161</v>
+      </c>
+      <c r="E87" t="s">
+        <v>173</v>
+      </c>
+      <c r="F87" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88">
+        <f>A87+1</f>
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>164</v>
+      </c>
+      <c r="C88">
+        <v>31</v>
+      </c>
+      <c r="D88" t="s">
+        <v>161</v>
+      </c>
+      <c r="E88" t="s">
+        <v>171</v>
+      </c>
+      <c r="F88" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89">
+        <f>A88+1</f>
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>164</v>
+      </c>
+      <c r="C89">
+        <v>32</v>
+      </c>
+      <c r="D89" t="s">
+        <v>161</v>
+      </c>
+      <c r="E89" t="s">
+        <v>43</v>
+      </c>
+      <c r="F89" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90">
+        <f>A89+1</f>
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>164</v>
+      </c>
+      <c r="C90">
+        <v>33</v>
+      </c>
+      <c r="D90" t="s">
+        <v>161</v>
+      </c>
+      <c r="E90" t="s">
+        <v>169</v>
+      </c>
+      <c r="F90" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91">
+        <f>A90+1</f>
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>164</v>
+      </c>
+      <c r="C91">
+        <v>34</v>
+      </c>
+      <c r="D91" t="s">
+        <v>161</v>
+      </c>
+      <c r="E91" t="s">
+        <v>168</v>
+      </c>
+      <c r="F91" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92">
+        <f>A91+1</f>
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>164</v>
+      </c>
+      <c r="C92">
+        <v>35</v>
+      </c>
+      <c r="D92" t="s">
+        <v>161</v>
+      </c>
+      <c r="E92" t="s">
+        <v>170</v>
+      </c>
+      <c r="F92" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93">
+        <f>A92+1</f>
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>164</v>
+      </c>
+      <c r="C93">
+        <v>36</v>
+      </c>
+      <c r="D93" t="s">
+        <v>161</v>
+      </c>
+      <c r="E93" t="s">
+        <v>171</v>
+      </c>
+      <c r="F93" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94">
+        <f>A93+1</f>
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>164</v>
+      </c>
+      <c r="C94">
+        <v>37</v>
+      </c>
+      <c r="D94" t="s">
+        <v>161</v>
+      </c>
+      <c r="E94" t="s">
+        <v>169</v>
+      </c>
+      <c r="F94" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95">
+        <f>A94+1</f>
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>164</v>
+      </c>
+      <c r="C95">
+        <v>38</v>
+      </c>
+      <c r="D95" t="s">
+        <v>161</v>
+      </c>
+      <c r="E95" t="s">
+        <v>168</v>
+      </c>
+      <c r="F95" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96">
+        <f>A95+1</f>
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>164</v>
+      </c>
+      <c r="C96">
+        <v>39</v>
+      </c>
+      <c r="D96" t="s">
+        <v>161</v>
+      </c>
+      <c r="E96" t="s">
+        <v>172</v>
+      </c>
+      <c r="F96" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97">
+        <f>A96+1</f>
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>164</v>
+      </c>
+      <c r="C97">
+        <v>40</v>
+      </c>
+      <c r="D97" t="s">
+        <v>161</v>
+      </c>
+      <c r="E97" t="s">
+        <v>173</v>
+      </c>
+      <c r="F97" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98">
+        <f>A97+1</f>
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>164</v>
+      </c>
+      <c r="C98">
+        <v>41</v>
+      </c>
+      <c r="D98" t="s">
+        <v>161</v>
+      </c>
+      <c r="E98" t="s">
+        <v>175</v>
+      </c>
+      <c r="F98" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99">
+        <f>A98+1</f>
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>164</v>
+      </c>
+      <c r="C99">
+        <v>28</v>
+      </c>
+      <c r="D99" t="s">
+        <v>161</v>
+      </c>
+      <c r="E99" t="s">
+        <v>174</v>
+      </c>
+      <c r="F99" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100">
+        <f>A99+1</f>
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>164</v>
+      </c>
+      <c r="C100">
+        <v>29</v>
+      </c>
+      <c r="D100" t="s">
+        <v>161</v>
+      </c>
+      <c r="E100" t="s">
+        <v>172</v>
+      </c>
+      <c r="F100" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101">
+        <f>A100+1</f>
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>164</v>
+      </c>
+      <c r="C101">
+        <v>30</v>
+      </c>
+      <c r="D101" t="s">
+        <v>161</v>
+      </c>
+      <c r="E101" t="s">
+        <v>173</v>
+      </c>
+      <c r="F101" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="F1:F101"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
media upload to cloudinary
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="200">
   <si>
     <t>tomyeh</t>
   </si>
@@ -559,6 +559,72 @@
   </si>
   <si>
     <t>Landmark</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>consent</t>
+  </si>
+  <si>
+    <t>I have consented</t>
+  </si>
+  <si>
+    <t>Tom Yeh</t>
+  </si>
+  <si>
+    <t>Abby Stangl</t>
+  </si>
+  <si>
+    <t>Mike Skirpan</t>
+  </si>
+  <si>
+    <t>Jose Meti</t>
+  </si>
+  <si>
+    <t>Matt Kesh</t>
+  </si>
+  <si>
+    <t>Jackie Hama</t>
+  </si>
+  <si>
+    <t>Carol Boston</t>
+  </si>
+  <si>
+    <t>Jenny Preece</t>
+  </si>
+  <si>
+    <t>Petter Joisterest</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>tom@mail.com</t>
+  </si>
+  <si>
+    <t>abby@mail.com</t>
+  </si>
+  <si>
+    <t>mike@mail.com</t>
+  </si>
+  <si>
+    <t>jose@mail.com</t>
+  </si>
+  <si>
+    <t>matt@mail.com</t>
+  </si>
+  <si>
+    <t>jackie@mail.com</t>
+  </si>
+  <si>
+    <t>carol@umd.edu</t>
+  </si>
+  <si>
+    <t>jenny@umd.edu</t>
+  </si>
+  <si>
+    <t>petter@umd.edu</t>
   </si>
 </sst>
 </file>
@@ -618,7 +684,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="136">
+  <cellStyleXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -755,12 +821,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="148"/>
   </cellXfs>
-  <cellStyles count="136">
+  <cellStyles count="149">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -855,6 +935,12 @@
     <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -896,6 +982,13 @@
     <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3991,95 +4084,231 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:6">
       <c r="A1">
         <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2">
+        <v>1234</v>
+      </c>
+      <c r="F2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3">
+        <v>1234</v>
+      </c>
+      <c r="F3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4">
+        <v>1234</v>
+      </c>
+      <c r="F4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5">
+        <v>1234</v>
+      </c>
+      <c r="F5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6">
+        <v>1234</v>
+      </c>
+      <c r="F6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7">
+        <v>1234</v>
+      </c>
+      <c r="F7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8">
+        <v>1234</v>
+      </c>
+      <c r="F8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9">
+        <v>1234</v>
+      </c>
+      <c r="F9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
       </c>
+      <c r="C10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10">
+        <v>1234</v>
+      </c>
+      <c r="F10" t="s">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -4094,7 +4323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add image_url to site
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="265">
   <si>
     <t>tomyeh</t>
   </si>
@@ -670,18 +670,12 @@
     <t>Pilot</t>
   </si>
   <si>
-    <t>Pilot test</t>
-  </si>
-  <si>
     <t>cu_design_idea</t>
   </si>
   <si>
     <t>Design Idea</t>
   </si>
   <si>
-    <t>Contribute your design idea</t>
-  </si>
-  <si>
     <t>aces_design_idea</t>
   </si>
   <si>
@@ -749,6 +743,84 @@
   </si>
   <si>
     <t>Like</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Stump the Community</t>
+  </si>
+  <si>
+    <t>Find an animal or plant that the NatureNet userbase won’t be able to name!</t>
+  </si>
+  <si>
+    <t>Pilot data from 2013</t>
+  </si>
+  <si>
+    <t>aces_stump</t>
+  </si>
+  <si>
+    <t>Find evidence of as many different kinds of bird or animal as you can!</t>
+  </si>
+  <si>
+    <t>Tracks</t>
+  </si>
+  <si>
+    <t>Native or Not?</t>
+  </si>
+  <si>
+    <t>Photograph an animal or plant that you know either is or isn’t indigenous to your region. If it’s not, try to tell us where it’s from!</t>
+  </si>
+  <si>
+    <t>aces_native</t>
+  </si>
+  <si>
+    <t>cu_stump</t>
+  </si>
+  <si>
+    <t>cu_tracks</t>
+  </si>
+  <si>
+    <t>aces_tracks</t>
+  </si>
+  <si>
+    <t>cu_native</t>
+  </si>
+  <si>
+    <t>umd_stump</t>
+  </si>
+  <si>
+    <t>umd_tracks</t>
+  </si>
+  <si>
+    <t>umd_native</t>
+  </si>
+  <si>
+    <t>uncc_stump</t>
+  </si>
+  <si>
+    <t>uncc_tracks</t>
+  </si>
+  <si>
+    <t>uncc_native</t>
+  </si>
+  <si>
+    <t>Contribute a design ideat to make NatureNet better</t>
+  </si>
+  <si>
+    <t>image_url</t>
+  </si>
+  <si>
+    <t>https://dl.dropboxusercontent.com/u/5104407/nntest/cu.jpg</t>
+  </si>
+  <si>
+    <t>https://dl.dropboxusercontent.com/u/5104407/nntest/aces.jpg</t>
+  </si>
+  <si>
+    <t>https://dl.dropboxusercontent.com/u/5104407/nntest/uncc.jpg</t>
+  </si>
+  <si>
+    <t>https://dl.dropboxusercontent.com/u/5104407/nntest/umd.jpg</t>
   </si>
 </sst>
 </file>
@@ -808,7 +880,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="218">
+  <cellStyleXfs count="229">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -958,6 +1030,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1033,7 +1116,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="148"/>
   </cellXfs>
-  <cellStyles count="218">
+  <cellStyles count="229">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1203,6 +1286,17 @@
     <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1582,8 +1676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K117"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5227,13 +5321,13 @@
         <v>12</v>
       </c>
       <c r="C110" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D110" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E110" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I110">
         <v>39.197670199999997</v>
@@ -5251,13 +5345,13 @@
         <v>14</v>
       </c>
       <c r="C111" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D111" t="s">
+        <v>229</v>
+      </c>
+      <c r="E111" t="s">
         <v>231</v>
-      </c>
-      <c r="E111" t="s">
-        <v>233</v>
       </c>
       <c r="I111">
         <v>39.197670199999997</v>
@@ -5275,13 +5369,13 @@
         <v>10</v>
       </c>
       <c r="C112" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D112" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E112" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I112">
         <v>39.197670199999997</v>
@@ -5299,13 +5393,13 @@
         <v>11</v>
       </c>
       <c r="C113" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D113" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E113" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I113">
         <v>39.197670199999997</v>
@@ -5323,13 +5417,13 @@
         <v>14</v>
       </c>
       <c r="C114" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D114" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E114" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I114">
         <v>39.197670199999997</v>
@@ -5347,13 +5441,13 @@
         <v>10</v>
       </c>
       <c r="C115" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D115" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E115" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I115">
         <v>39.197670199999997</v>
@@ -5371,13 +5465,13 @@
         <v>11</v>
       </c>
       <c r="C116" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D116" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E116" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I116">
         <v>39.197670199999997</v>
@@ -5395,13 +5489,13 @@
         <v>15</v>
       </c>
       <c r="C117" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D117" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E117" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I117">
         <v>39.197670199999997</v>
@@ -5459,7 +5553,7 @@
         <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -5482,7 +5576,7 @@
         <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -5505,7 +5599,7 @@
         <v>58</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5528,7 +5622,7 @@
         <v>58</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5551,7 +5645,7 @@
         <v>58</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5574,7 +5668,7 @@
         <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5597,7 +5691,7 @@
         <v>58</v>
       </c>
       <c r="G7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5620,7 +5714,7 @@
         <v>58</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -5643,7 +5737,7 @@
         <v>58</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5666,7 +5760,7 @@
         <v>58</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -5689,7 +5783,7 @@
         <v>58</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -5712,7 +5806,7 @@
         <v>58</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -5749,24 +5843,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="60.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -5789,7 +5883,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>213</v>
       </c>
       <c r="C2" t="s">
         <v>209</v>
@@ -5809,7 +5903,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
         <v>210</v>
@@ -5829,7 +5923,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>213</v>
       </c>
       <c r="C4" t="s">
         <v>212</v>
@@ -5838,7 +5932,7 @@
         <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>214</v>
+        <v>242</v>
       </c>
       <c r="F4" t="s">
         <v>83</v>
@@ -5849,16 +5943,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>239</v>
       </c>
       <c r="C5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5" t="s">
         <v>215</v>
       </c>
-      <c r="D5" t="s">
-        <v>216</v>
-      </c>
       <c r="E5" t="s">
-        <v>217</v>
+        <v>259</v>
       </c>
       <c r="F5" t="s">
         <v>81</v>
@@ -5869,16 +5963,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>239</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E6" t="s">
-        <v>217</v>
+        <v>259</v>
       </c>
       <c r="F6" t="s">
         <v>83</v>
@@ -5889,16 +5983,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>239</v>
       </c>
       <c r="C7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" t="s">
         <v>215</v>
       </c>
-      <c r="D7" t="s">
-        <v>216</v>
-      </c>
       <c r="E7" t="s">
-        <v>217</v>
+        <v>259</v>
       </c>
       <c r="F7" t="s">
         <v>79</v>
@@ -5909,18 +6003,269 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C8" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" t="s">
+        <v>215</v>
+      </c>
+      <c r="E8" t="s">
+        <v>259</v>
+      </c>
+      <c r="F8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>55</v>
       </c>
-      <c r="C8" t="s">
-        <v>219</v>
-      </c>
-      <c r="D8" t="s">
-        <v>216</v>
-      </c>
-      <c r="E8" t="s">
-        <v>217</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="C9" t="s">
+        <v>243</v>
+      </c>
+      <c r="D9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E9" t="s">
+        <v>241</v>
+      </c>
+      <c r="F9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <f>A9+1</f>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D10" t="s">
+        <v>245</v>
+      </c>
+      <c r="E10" t="s">
+        <v>244</v>
+      </c>
+      <c r="F10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <f t="shared" ref="A11:A20" si="0">A10+1</f>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>248</v>
+      </c>
+      <c r="D11" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>249</v>
+      </c>
+      <c r="D12" t="s">
+        <v>240</v>
+      </c>
+      <c r="E12" t="s">
+        <v>241</v>
+      </c>
+      <c r="F12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D13" t="s">
+        <v>245</v>
+      </c>
+      <c r="E13" t="s">
+        <v>244</v>
+      </c>
+      <c r="F13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>252</v>
+      </c>
+      <c r="D14" t="s">
+        <v>246</v>
+      </c>
+      <c r="E14" t="s">
+        <v>247</v>
+      </c>
+      <c r="F14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>253</v>
+      </c>
+      <c r="D15" t="s">
+        <v>240</v>
+      </c>
+      <c r="E15" t="s">
+        <v>241</v>
+      </c>
+      <c r="F15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>254</v>
+      </c>
+      <c r="D16" t="s">
+        <v>245</v>
+      </c>
+      <c r="E16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
+        <v>255</v>
+      </c>
+      <c r="D17" t="s">
+        <v>246</v>
+      </c>
+      <c r="E17" t="s">
+        <v>247</v>
+      </c>
+      <c r="F17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>256</v>
+      </c>
+      <c r="D18" t="s">
+        <v>240</v>
+      </c>
+      <c r="E18" t="s">
+        <v>241</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>257</v>
+      </c>
+      <c r="D19" t="s">
+        <v>245</v>
+      </c>
+      <c r="E19" t="s">
+        <v>244</v>
+      </c>
+      <c r="F19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" t="s">
+        <v>246</v>
+      </c>
+      <c r="E20" t="s">
+        <v>247</v>
+      </c>
+      <c r="F20" t="s">
         <v>80</v>
       </c>
     </row>
@@ -5939,7 +6284,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -8161,7 +8508,7 @@
         <v>106</v>
       </c>
       <c r="D106" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F106" t="s">
         <v>1</v>
@@ -8179,7 +8526,7 @@
         <v>107</v>
       </c>
       <c r="D107" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F107" t="s">
         <v>1</v>
@@ -8197,7 +8544,7 @@
         <v>108</v>
       </c>
       <c r="D108" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F108" t="s">
         <v>1</v>
@@ -8215,7 +8562,7 @@
         <v>110</v>
       </c>
       <c r="D109" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F109" t="s">
         <v>14</v>
@@ -8233,7 +8580,7 @@
         <v>111</v>
       </c>
       <c r="D110" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F110" t="s">
         <v>14</v>
@@ -8251,7 +8598,7 @@
         <v>112</v>
       </c>
       <c r="D111" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F111" t="s">
         <v>14</v>
@@ -8269,7 +8616,7 @@
         <v>113</v>
       </c>
       <c r="D112" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F112" t="s">
         <v>14</v>
@@ -8289,10 +8636,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8301,7 +8648,7 @@
     <col min="3" max="3" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>5</v>
       </c>
@@ -8311,8 +8658,11 @@
       <c r="C1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8323,7 +8673,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8333,8 +8683,11 @@
       <c r="C3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -8344,8 +8697,11 @@
       <c r="C4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8355,8 +8711,11 @@
       <c r="C5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -8366,8 +8725,16 @@
       <c r="C6" t="s">
         <v>86</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>264</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
api note includes feedbacks
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2480" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="317">
   <si>
     <t>tomyeh</t>
   </si>
@@ -841,12 +841,6 @@
     <t>It's time to meet ACES' resident Golden Eagle, a real Aspen local. In the summer of 1982 this eagle was found on the backside of Aspen Mountain by hikers.  She was brought to a raptor rehabilitation center in Fort Collins, where she was treated for a broken right wing and left leg. She was then returned to Aspen and Hallam Lake where she has lived ever since.</t>
   </si>
   <si>
-    <t>{"latitude": 39.195216, "longitude": -106.821265}</t>
-  </si>
-  <si>
-    <t>{"latitude": 39.195428,"longitude": -106.822069}</t>
-  </si>
-  <si>
     <t>1. Hub of Activities</t>
   </si>
   <si>
@@ -889,42 +883,27 @@
     <t>Beavers have been living here at Hallam Lake for many decades. They are most active at dawn and dusk. Do you see any signs of their activity? Chewed sticks, pointed tree stumps, dams, and lodges are all clues that beavers live nearby. The beavers here live in a bank lodge located on the other side of the lake, under the leaning blue spruce tree.</t>
   </si>
   <si>
-    <t>{"latitude": 39.195798,"longitude": -106.822166}</t>
-  </si>
-  <si>
     <t>5. Outdoor Classroom</t>
   </si>
   <si>
     <t>As you stand here at the teaching platforms, you are joining a long lineage of visitors who have found Hallam Lake a place of connection and inspiration. Since the very early days of ACES, children and adults have used this spot as an outdoor classroom and laboratory, a place of thoughtful observation and study to reconnect with nature. Artists and writers have used Hallam Lake as an outdoor studio, finding these platforms to be a wonderful spot to express themselves. If you have a camera, a journal, or watercolors, stop and get in touch with your inner artist!</t>
   </si>
   <si>
-    <t>{"latitude": 39.195998,"longitude": -106.821823}</t>
-  </si>
-  <si>
     <t>6. Powerful Ties from Past to Present</t>
   </si>
   <si>
     <t>Look down and take notice of the strange plants growing next to the trail. The plants below are commonly known as horsetails and are a connection to an ancient part of plant history. Spore-producing horsetails belong to the genus Equisetum, in a plant family that is over 300 million years old!  They are also called scouring rushes because silica, stored in the plant's cells, makes them effective for scrubbing pots or polishing wood.  Native Americans used the horsetails as a blood coagulant, and more recent medical research has shown these plants to be an effective diuretic.  Can you think of other ancient plants or animals that are still living today?</t>
   </si>
   <si>
-    <t>{"latitude": 39.19643,"longitude": -106.821629}</t>
-  </si>
-  <si>
     <t>7. Overlook the Sanctuary</t>
   </si>
   <si>
     <t>Turn left for an out-and-back to the marsh platform.</t>
   </si>
   <si>
-    <t>{"latitude": 39.196613,"longitude": -106.82156}</t>
-  </si>
-  <si>
     <t>8. Bird Hollow</t>
   </si>
   <si>
-    <t>{"latitude": 39.196513,"longitude": -106.821265}</t>
-  </si>
-  <si>
     <t>9. Where Rivers Come Together</t>
   </si>
   <si>
@@ -934,18 +913,12 @@
     <t>The rushing water below is the Roaring Fork River just before it meets Hunter Creek. Hallam Lake can be geographically defined as the low, wet riparian area adjacent to the confluence of Hunter Creek and the Roaring Fork River.</t>
   </si>
   <si>
-    <t>{"latitude": 39.196368,"longitude": -106.821265}</t>
-  </si>
-  <si>
     <t>10. Birds of Prey</t>
   </si>
   <si>
     <t>You are standing in front of the Birds of Prey (BOP) House, the hub of our non-releasable raptor program. While at ACES, the resident BOP serve as our best educators, allowing visitors to get up close and personal to powerful wild animals.</t>
   </si>
   <si>
-    <t>{"latitude": 39.195324,"longitude": -106.821227}</t>
-  </si>
-  <si>
     <t>aces_landmark11</t>
   </si>
   <si>
@@ -955,7 +928,55 @@
     <t>Thank you for visiting Hallam Lake today! This has always been a place of connection for animals and people, from the early times of the Ute Indians to the present-day visitors and guests of our nature center. Birds touch down on the lake and rest, and this is a safe haven for deer, black bears, and beavers to raise their young. Hallam Lake is an important hub for the Aspen community, offering a place for people to share stories and ideas, as well as find inspiration and peace. Nature centers in many communities provide a place where everyone is welcome regardless of race, religion, or financial status.</t>
   </si>
   <si>
-    <t>{"latitude": 39.195241,"longitude": -106.82112}</t>
+    <t>umd_landmark_hcil</t>
+  </si>
+  <si>
+    <t>HCIL</t>
+  </si>
+  <si>
+    <t>Human Computer Interaction Laboratory</t>
+  </si>
+  <si>
+    <t>AV Williams</t>
+  </si>
+  <si>
+    <t>AV Williams, Computer Science, UMIACS</t>
+  </si>
+  <si>
+    <t>umd_landmark_avw</t>
+  </si>
+  <si>
+    <t>McKeldin Mall</t>
+  </si>
+  <si>
+    <t>umd_landmark_mall</t>
+  </si>
+  <si>
+    <t>Woodward Hall</t>
+  </si>
+  <si>
+    <t>Woordward Hall</t>
+  </si>
+  <si>
+    <t>uncc_landmark_woodward</t>
+  </si>
+  <si>
+    <t>cu_landmark_dlc</t>
+  </si>
+  <si>
+    <t>Discovery Learning Center</t>
+  </si>
+  <si>
+    <t>DLC</t>
+  </si>
+  <si>
+    <t>C4C - Center for Community</t>
+  </si>
+  <si>
+    <t>Center for Community</t>
+  </si>
+  <si>
+    <t>cu_landmark_c4c</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1036,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="241">
+  <cellStyleXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1165,6 +1186,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1263,7 +1292,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="148"/>
   </cellXfs>
-  <cellStyles count="241">
+  <cellStyles count="249">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1456,6 +1485,14 @@
     <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6002,9 +6039,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -6017,7 +6056,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -6345,7 +6384,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -6366,7 +6405,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -6387,7 +6426,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -6408,7 +6447,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -6429,7 +6468,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6441,7 +6480,7 @@
         <v>267</v>
       </c>
       <c r="D21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E21" t="s">
         <v>269</v>
@@ -6449,11 +6488,14 @@
       <c r="F21" t="s">
         <v>83</v>
       </c>
-      <c r="G21" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="G21">
+        <v>39.195</v>
+      </c>
+      <c r="H21">
+        <v>-106.821141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -6465,7 +6507,7 @@
         <v>268</v>
       </c>
       <c r="D22" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E22" t="s">
         <v>270</v>
@@ -6473,11 +6515,14 @@
       <c r="F22" t="s">
         <v>83</v>
       </c>
-      <c r="G22" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="G22">
+        <v>39.195008000000001</v>
+      </c>
+      <c r="H22">
+        <v>-106.82138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -6486,22 +6531,25 @@
         <v>266</v>
       </c>
       <c r="C23" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D23" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E23" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F23" t="s">
         <v>83</v>
       </c>
-      <c r="G23" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="G23">
+        <v>39.195428</v>
+      </c>
+      <c r="H23">
+        <v>-106.822069</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -6510,22 +6558,25 @@
         <v>266</v>
       </c>
       <c r="C24" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D24" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E24" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F24" t="s">
         <v>83</v>
       </c>
-      <c r="G24" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="G24">
+        <v>39.195798000000003</v>
+      </c>
+      <c r="H24">
+        <v>-106.822166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -6534,22 +6585,25 @@
         <v>266</v>
       </c>
       <c r="C25" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D25" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E25" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F25" t="s">
         <v>83</v>
       </c>
-      <c r="G25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="G25">
+        <v>39.195998000000003</v>
+      </c>
+      <c r="H25">
+        <v>-106.82182299999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -6558,22 +6612,25 @@
         <v>266</v>
       </c>
       <c r="C26" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D26" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E26" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F26" t="s">
         <v>83</v>
       </c>
-      <c r="G26" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="G26">
+        <v>39.196429999999999</v>
+      </c>
+      <c r="H26">
+        <v>-106.821629</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -6582,22 +6639,25 @@
         <v>266</v>
       </c>
       <c r="C27" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D27" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E27" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F27" t="s">
         <v>83</v>
       </c>
-      <c r="G27" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="G27">
+        <v>39.196612999999999</v>
+      </c>
+      <c r="H27">
+        <v>-106.82156000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -6606,22 +6666,25 @@
         <v>266</v>
       </c>
       <c r="C28" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D28" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E28" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="F28" t="s">
         <v>83</v>
       </c>
-      <c r="G28" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="G28">
+        <v>39.196513000000003</v>
+      </c>
+      <c r="H28">
+        <v>-106.521265</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -6630,22 +6693,25 @@
         <v>266</v>
       </c>
       <c r="C29" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D29" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="E29" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="F29" t="s">
         <v>83</v>
       </c>
-      <c r="G29" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="G29">
+        <v>39.196368</v>
+      </c>
+      <c r="H29">
+        <v>-106.821265</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -6654,22 +6720,25 @@
         <v>266</v>
       </c>
       <c r="C30" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D30" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="E30" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="F30" t="s">
         <v>83</v>
       </c>
-      <c r="G30" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="G30">
+        <v>39.195323999999999</v>
+      </c>
+      <c r="H30">
+        <v>-106.82122699999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -6678,19 +6747,178 @@
         <v>266</v>
       </c>
       <c r="C31" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="D31" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="E31" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="F31" t="s">
         <v>83</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31">
+        <v>39.195216000000002</v>
+      </c>
+      <c r="H31">
+        <v>-106.821004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>266</v>
+      </c>
+      <c r="C32" t="s">
+        <v>300</v>
+      </c>
+      <c r="D32" t="s">
+        <v>301</v>
+      </c>
+      <c r="E32" t="s">
+        <v>302</v>
+      </c>
+      <c r="F32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G32">
+        <v>39.987901000000001</v>
+      </c>
+      <c r="H32">
+        <v>-76.941598999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>266</v>
+      </c>
+      <c r="C33" t="s">
+        <v>305</v>
+      </c>
+      <c r="D33" t="s">
+        <v>303</v>
+      </c>
+      <c r="E33" t="s">
+        <v>304</v>
+      </c>
+      <c r="F33" t="s">
+        <v>79</v>
+      </c>
+      <c r="G33">
+        <v>38.990752000000001</v>
+      </c>
+      <c r="H33">
+        <v>-76.936271000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>266</v>
+      </c>
+      <c r="C34" t="s">
+        <v>307</v>
+      </c>
+      <c r="D34" t="s">
+        <v>306</v>
+      </c>
+      <c r="E34" t="s">
+        <v>306</v>
+      </c>
+      <c r="F34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34">
+        <v>38.987133999999998</v>
+      </c>
+      <c r="H34">
+        <v>-76.940305899999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>266</v>
+      </c>
+      <c r="C35" t="s">
+        <v>310</v>
+      </c>
+      <c r="D35" t="s">
         <v>309</v>
+      </c>
+      <c r="E35" t="s">
+        <v>308</v>
+      </c>
+      <c r="F35" t="s">
+        <v>80</v>
+      </c>
+      <c r="G35">
+        <v>35.307238699999999</v>
+      </c>
+      <c r="H35">
+        <v>-80.735332299999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>266</v>
+      </c>
+      <c r="C36" t="s">
+        <v>311</v>
+      </c>
+      <c r="D36" t="s">
+        <v>312</v>
+      </c>
+      <c r="E36" t="s">
+        <v>313</v>
+      </c>
+      <c r="F36" t="s">
+        <v>81</v>
+      </c>
+      <c r="G36">
+        <v>40.007613999999997</v>
+      </c>
+      <c r="H36">
+        <v>-105.261771</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>266</v>
+      </c>
+      <c r="C37" t="s">
+        <v>316</v>
+      </c>
+      <c r="D37" t="s">
+        <v>315</v>
+      </c>
+      <c r="E37" t="s">
+        <v>314</v>
+      </c>
+      <c r="F37" t="s">
+        <v>81</v>
+      </c>
+      <c r="G37">
+        <v>40.004443000000002</v>
+      </c>
+      <c r="H37">
+        <v>-105.26484000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sync feedback on context
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2480" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="318">
   <si>
     <t>tomyeh</t>
   </si>
@@ -977,6 +977,9 @@
   </si>
   <si>
     <t>cu_landmark_c4c</t>
+  </si>
+  <si>
+    <t>Context</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1039,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="249">
+  <cellStyleXfs count="251">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1186,6 +1189,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1292,7 +1297,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="148"/>
   </cellXfs>
-  <cellStyles count="249">
+  <cellStyles count="251">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1493,6 +1498,8 @@
     <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6041,8 +6048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6934,11 +6941,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F112"/>
+  <dimension ref="A1:F116"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -6952,7 +6957,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
         <v>39</v>
@@ -9272,6 +9277,74 @@
       </c>
       <c r="F112" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>317</v>
+      </c>
+      <c r="C113">
+        <v>8</v>
+      </c>
+      <c r="D113" t="s">
+        <v>238</v>
+      </c>
+      <c r="F113" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>317</v>
+      </c>
+      <c r="C114">
+        <v>9</v>
+      </c>
+      <c r="D114" t="s">
+        <v>238</v>
+      </c>
+      <c r="F114" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>317</v>
+      </c>
+      <c r="C115">
+        <v>10</v>
+      </c>
+      <c r="D115" t="s">
+        <v>238</v>
+      </c>
+      <c r="F115" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>317</v>
+      </c>
+      <c r="C116">
+        <v>11</v>
+      </c>
+      <c r="D116" t="s">
+        <v>238</v>
+      </c>
+      <c r="F116" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed timestamp -> utc
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="2480" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="1" r:id="rId1"/>
@@ -1039,7 +1039,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="251">
+  <cellStyleXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1189,6 +1189,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1297,7 +1299,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="148"/>
   </cellXfs>
-  <cellStyles count="251">
+  <cellStyles count="253">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1500,6 +1502,8 @@
     <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1879,8 +1883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K117"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="F117" sqref="F117"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1945,10 +1949,10 @@
         <v>98</v>
       </c>
       <c r="I2">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J2">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1977,10 +1981,10 @@
         <v>99</v>
       </c>
       <c r="I3">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J3">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2009,10 +2013,10 @@
         <v>100</v>
       </c>
       <c r="I4">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J4">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2041,10 +2045,10 @@
         <v>101</v>
       </c>
       <c r="I5">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J5">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2073,10 +2077,10 @@
         <v>102</v>
       </c>
       <c r="I6">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J6">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2105,10 +2109,10 @@
         <v>103</v>
       </c>
       <c r="I7">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J7">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2137,10 +2141,10 @@
         <v>104</v>
       </c>
       <c r="I8">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J8">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2170,10 +2174,10 @@
         <v>105</v>
       </c>
       <c r="I9">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J9">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2203,10 +2207,10 @@
         <v>106</v>
       </c>
       <c r="I10">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J10">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2236,10 +2240,10 @@
         <v>107</v>
       </c>
       <c r="I11">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J11">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -2269,10 +2273,10 @@
         <v>108</v>
       </c>
       <c r="I12">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J12">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -2302,10 +2306,10 @@
         <v>109</v>
       </c>
       <c r="I13">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J13">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -2335,10 +2339,10 @@
         <v>110</v>
       </c>
       <c r="I14">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J14">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -2368,10 +2372,10 @@
         <v>111</v>
       </c>
       <c r="I15">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J15">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2401,10 +2405,10 @@
         <v>112</v>
       </c>
       <c r="I16">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J16">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2434,10 +2438,10 @@
         <v>113</v>
       </c>
       <c r="I17">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J17">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -2467,10 +2471,10 @@
         <v>114</v>
       </c>
       <c r="I18">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J18">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2500,10 +2504,10 @@
         <v>115</v>
       </c>
       <c r="I19">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J19">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2533,10 +2537,10 @@
         <v>116</v>
       </c>
       <c r="I20">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J20">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2566,10 +2570,10 @@
         <v>117</v>
       </c>
       <c r="I21">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J21">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -2599,10 +2603,10 @@
         <v>118</v>
       </c>
       <c r="I22">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J22">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2632,10 +2636,10 @@
         <v>119</v>
       </c>
       <c r="I23">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J23">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2665,10 +2669,10 @@
         <v>120</v>
       </c>
       <c r="I24">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J24">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2698,10 +2702,10 @@
         <v>121</v>
       </c>
       <c r="I25">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J25">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2731,10 +2735,10 @@
         <v>122</v>
       </c>
       <c r="I26">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J26">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2764,10 +2768,10 @@
         <v>123</v>
       </c>
       <c r="I27">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J27">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2797,10 +2801,10 @@
         <v>124</v>
       </c>
       <c r="I28">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J28">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2830,10 +2834,10 @@
         <v>125</v>
       </c>
       <c r="I29">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J29">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2863,10 +2867,10 @@
         <v>126</v>
       </c>
       <c r="I30">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J30">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2896,10 +2900,10 @@
         <v>127</v>
       </c>
       <c r="I31">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J31">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2929,10 +2933,10 @@
         <v>128</v>
       </c>
       <c r="I32">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J32">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2962,10 +2966,10 @@
         <v>129</v>
       </c>
       <c r="I33">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J33">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2995,10 +2999,10 @@
         <v>130</v>
       </c>
       <c r="I34">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J34">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -3028,10 +3032,10 @@
         <v>131</v>
       </c>
       <c r="I35">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J35">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -3061,10 +3065,10 @@
         <v>132</v>
       </c>
       <c r="I36">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J36">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -3094,10 +3098,10 @@
         <v>133</v>
       </c>
       <c r="I37">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J37">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -3127,10 +3131,10 @@
         <v>134</v>
       </c>
       <c r="I38">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J38">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -3160,10 +3164,10 @@
         <v>135</v>
       </c>
       <c r="I39">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J39">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -3193,10 +3197,10 @@
         <v>136</v>
       </c>
       <c r="I40">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J40">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -3226,10 +3230,10 @@
         <v>137</v>
       </c>
       <c r="I41">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J41">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -3259,10 +3263,10 @@
         <v>138</v>
       </c>
       <c r="I42">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J42">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -3292,10 +3296,10 @@
         <v>139</v>
       </c>
       <c r="I43">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J43">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -3325,10 +3329,10 @@
         <v>140</v>
       </c>
       <c r="I44">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J44">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -3358,10 +3362,10 @@
         <v>141</v>
       </c>
       <c r="I45">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J45">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -3391,10 +3395,10 @@
         <v>142</v>
       </c>
       <c r="I46">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J46">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -3424,10 +3428,10 @@
         <v>143</v>
       </c>
       <c r="I47">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J47">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -3457,10 +3461,10 @@
         <v>144</v>
       </c>
       <c r="I48">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J48">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -3490,10 +3494,10 @@
         <v>145</v>
       </c>
       <c r="I49">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J49">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -3523,10 +3527,10 @@
         <v>146</v>
       </c>
       <c r="I50">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J50">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -3556,10 +3560,10 @@
         <v>147</v>
       </c>
       <c r="I51">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J51">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -3589,10 +3593,10 @@
         <v>148</v>
       </c>
       <c r="I52">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J52">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -3622,10 +3626,10 @@
         <v>149</v>
       </c>
       <c r="I53">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J53">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -3655,10 +3659,10 @@
         <v>150</v>
       </c>
       <c r="I54">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J54">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -3688,10 +3692,10 @@
         <v>151</v>
       </c>
       <c r="I55">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J55">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -3721,10 +3725,10 @@
         <v>152</v>
       </c>
       <c r="I56">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J56">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -3754,10 +3758,10 @@
         <v>153</v>
       </c>
       <c r="I57">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J57">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -3787,10 +3791,10 @@
         <v>154</v>
       </c>
       <c r="I58">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J58">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -3820,10 +3824,10 @@
         <v>155</v>
       </c>
       <c r="I59">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J59">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -3853,10 +3857,10 @@
         <v>156</v>
       </c>
       <c r="I60">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J60">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -3886,10 +3890,10 @@
         <v>157</v>
       </c>
       <c r="I61">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J61">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -3919,10 +3923,10 @@
         <v>158</v>
       </c>
       <c r="I62">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J62">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -3952,10 +3956,10 @@
         <v>159</v>
       </c>
       <c r="I63">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J63">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -3985,10 +3989,10 @@
         <v>160</v>
       </c>
       <c r="I64">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J64">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -4018,10 +4022,10 @@
         <v>161</v>
       </c>
       <c r="I65">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J65">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -4051,10 +4055,10 @@
         <v>162</v>
       </c>
       <c r="I66">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J66">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -4084,10 +4088,10 @@
         <v>163</v>
       </c>
       <c r="I67">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J67">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -4117,10 +4121,10 @@
         <v>164</v>
       </c>
       <c r="I68">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J68">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -4150,10 +4154,10 @@
         <v>165</v>
       </c>
       <c r="I69">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J69">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -4183,10 +4187,10 @@
         <v>166</v>
       </c>
       <c r="I70">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J70">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -4216,10 +4220,10 @@
         <v>167</v>
       </c>
       <c r="I71">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J71">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -4249,10 +4253,10 @@
         <v>168</v>
       </c>
       <c r="I72">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J72">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -4282,10 +4286,10 @@
         <v>169</v>
       </c>
       <c r="I73">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J73">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -4315,10 +4319,10 @@
         <v>170</v>
       </c>
       <c r="I74">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J74">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -4348,10 +4352,10 @@
         <v>171</v>
       </c>
       <c r="I75">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J75">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -4381,10 +4385,10 @@
         <v>172</v>
       </c>
       <c r="I76">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J76">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -4414,10 +4418,10 @@
         <v>173</v>
       </c>
       <c r="I77">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J77">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -4447,10 +4451,10 @@
         <v>174</v>
       </c>
       <c r="I78">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J78">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -4480,10 +4484,10 @@
         <v>175</v>
       </c>
       <c r="I79">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J79">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -4513,10 +4517,10 @@
         <v>176</v>
       </c>
       <c r="I80">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J80">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -4546,10 +4550,10 @@
         <v>177</v>
       </c>
       <c r="I81">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J81">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -4579,10 +4583,10 @@
         <v>178</v>
       </c>
       <c r="I82">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J82">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -4612,10 +4616,10 @@
         <v>179</v>
       </c>
       <c r="I83">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J83">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -4645,10 +4649,10 @@
         <v>180</v>
       </c>
       <c r="I84">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J84">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -4678,10 +4682,10 @@
         <v>181</v>
       </c>
       <c r="I85">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J85">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -4711,10 +4715,10 @@
         <v>182</v>
       </c>
       <c r="I86">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J86">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -4744,10 +4748,10 @@
         <v>183</v>
       </c>
       <c r="I87">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J87">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -4777,10 +4781,10 @@
         <v>184</v>
       </c>
       <c r="I88">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J88">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -4810,10 +4814,10 @@
         <v>185</v>
       </c>
       <c r="I89">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J89">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -4843,10 +4847,10 @@
         <v>186</v>
       </c>
       <c r="I90">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J90">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -4876,10 +4880,10 @@
         <v>187</v>
       </c>
       <c r="I91">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J91">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -4909,10 +4913,10 @@
         <v>188</v>
       </c>
       <c r="I92">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J92">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -4942,10 +4946,10 @@
         <v>189</v>
       </c>
       <c r="I93">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J93">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -4975,10 +4979,10 @@
         <v>190</v>
       </c>
       <c r="I94">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J94">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -5008,10 +5012,10 @@
         <v>191</v>
       </c>
       <c r="I95">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J95">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -5041,10 +5045,10 @@
         <v>192</v>
       </c>
       <c r="I96">
-        <v>39.197670199999997</v>
+        <v>39.195794999999997</v>
       </c>
       <c r="J96">
-        <v>-106.8210536</v>
+        <v>-106.82182899999999</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -6943,7 +6947,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>